<commit_message>
Proceeded with the campaign, added battle handling
</commit_message>
<xml_diff>
--- a/Кампания.xlsx
+++ b/Кампания.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usеr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usеr\source\repos\DungeonsAndGPTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E11666E-346B-4C2F-A906-209A96F4403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A47E9A9-C1E8-4DDF-82C8-C69806FE3B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{2157F66B-6B78-45F2-A854-EF263FAA889B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{2157F66B-6B78-45F2-A854-EF263FAA889B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="91">
   <si>
     <t>Этап</t>
   </si>
@@ -1239,6 +1239,123 @@
 В этот момент Мудрецы Звезд подняли свои посохи вверх, создавая защитный барьер вокруг Осириса. Вихрь световой энергии, который он вызвал, стал контролируемым и начал вращаться вокруг него, словно звездные орбиты, создавая защитный щит.
 "Осирис, тебе предстоит пройти через испытания Звездного Резонанса, чтобы раскрыть истинный потенциал своей магии и спасти Эльдорию от тьмы. С этого момента ты несешь бремя не только своей судьбы, но и судьбы всего мира," объявил старший из Мудрецов Звезд.
 Игроку предстояло взять в руки свой Звездный посох, облачиться в Драконью чешую и взглянуть на светящийся вихрь световой энергии. Следы Звезд на его драконьей чешуе мерцали, свидетельствуя о его соединении с звездной энергией. Теперь, с магией и знаниями, полученными от Мудрецов Звезд, Осирис был готов к финальной битве, которая должна была решить судьбу Эльдории.</t>
+  </si>
+  <si>
+    <t>Вот вся информация о мире, персонаже, его навыках и предметах: *все дб*. В данной ситуации игрок выбрал "Произвести Звездный Взрыв, вызвав световой вихрь в Звездных Сферах.". Опиши, как финальный босс прервал это действие и начни сражение с ним.
+Можешь описать босса и его действия, однако действовать за игрока не надо. У игрока должно быть время ответить на любые действия босса.</t>
+  </si>
+  <si>
+    <t>Сияющая Астральная Платформа наполнилась светом звезд, когда Осирис поднял свой Звездный посох, готовясь к могущественному Звездному Взрыву. Звезды вокруг него начали колебаться, создавая вихрь световой энергии. Осирис сфокусировался, готовясь выпустить этот мощный магический удар.
+Внезапно, из темного портала возник фигура, высокая и величественная. Это был финальный босс - Теневой Хранитель, владыка Тени Забытых Богов. Его темные доспехи сверкали мистическим светом, а его глаза излучали ауру могущества.
+Теневой Хранитель поднял руку, прерывая Звездный Взрыв Осириса своим магическим щитом. Световой вихрь замер, и затем исчез в темной ауре вокруг босса. Хранитель произнес таинственные слова, вызывая волну тьмы, которая окутала Осириса.
+"Ты, драконид, слишком дерзок, пытаясь использовать звездную энергию против меня," грозно произнес Теневой Хранитель. "Теперь ты станешь свидетелем истинной мощи тьмы."
+Сражение началось. Теневой Хранитель с легкостью избегал атак Осириса, создавая магические барьеры и вызывая теневых слуг, чтобы помешать его действиям. Он использовал свою Чарующую Тьму, чтобы ослепить Осириса, и активировал временные ловушки, чтобы замедлить его движения.
+Осирис, обуреваемый тьмой, осознал, что ему нужно пристально изучить тактику босса и использовать свои навыки мудро. Теневой Хранитель был могучим противником, и каждый шаг игрока требовал внимательного обдумывания.
+В это время, внутри Осириса, Звездный Резонанс начал проявляться, предоставляя ему новые способности и возможности. Осирису предстояло разгадать тайны этого боя, чтобы использовать свою уникальную связь с звездами и драконьей силой для победы.</t>
+  </si>
+  <si>
+    <t>BattleLog</t>
+  </si>
+  <si>
+    <t>{
+  "BattleLog": {
+    "Enemies": [
+      {
+        "Name": "Теневой Хранитель",
+        "State": "Живой",
+        "Skills": [
+          "Магический Щит",
+          "Чарующая Тьма",
+          "Вызов Теневых Слуг",
+          "Активация Ловушек"
+        ],
+        "PossibleLoot": "Мистический Артефакт Тьмы",
+        "PerformedActions": []
+      }
+    ],
+    "PlayerActions": [],
+    "MainEvents": [
+      "Осирис готовится к Звездному Взрыву",
+      "Теневой Хранитель прерывает атаку магическим щитом",
+      "Хранитель вызывает тьму, окутывающую Осириса",
+      "Начало сражения с Теневым Хранителем"
+    ]
+  }
+}</t>
+  </si>
+  <si>
+    <t>Вот красочное описание начала сцены боя: *предыдущий output gpt*
+На основании этого верни json в следующем формате:
+```json
+{
+  "BattleLog":{
+    "Enemies":[
+      "Name":,
+      "State",
+      "Skills",
+      "PossibleLoot",
+      "PerformedActions"
+    ],
+    "PlayerActions":[],
+    "MainEvents":[]
+  }
+}
+```
+где в массиве Enemies записаны все враги игрока (самого игрока в этот список вносить не нужно, как и его союзников), в PlayerActions предпринятые игроком за время боя действия, а в MainEvents очень кратко пересказаны общие события сражения.</t>
+  </si>
+  <si>
+    <t>Вот описание мира, персонажа и его навыков, а также предыдущий лог боя:
+*SI, CS, CCS, WAC, BL* На основании этого предложи 3 новых варианта действий персонажа Осирис (они не должны повторять уже существующие, а так же все они должны быть направлены на атаку врагов, покидать локацию и бой нельзя) и выдай их в следующем виде:
+```json
+{
+  "PossibleActions":[
+    "",
+    "",
+    ""
+  ]
+}
+```</t>
+  </si>
+  <si>
+    <t>{
+  "PossibleActions": [
+    "Применить Звездный Резонанс для создания магического барьера, защищающего от магических атак Теневого Хранителя.",
+    "Использовать Цветущее Прозрение, чтобы обнаружить уязвимости в магическом облике Теневого Хранителя и атаковать его слабые места.",
+    "Активировать Хрономантический Переход для быстрого перемещения вокруг Теневого Хранителя и избежания его ловушек, затем совершить магическую атаку."
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Вот вся информация о мире, персонаже, его навыках: *БД ShortInfo, БД CharacterSkills - CharacterSkills.BeautifulDescription, CurrentCharacterState.
+В данной ситуации игрок хочет успешно совершил следующее действие: Активировать Хрономантический Переход для быстрого перемещения вокруг Теневого Хранителя и избежания его ловушек, затем совершить магическую атаку. Красочно, но немногословно (в один абзац), опиши, как это произошло. Учти, что описать нужно только предпринятое игроком действие и его последствия, додумывать дополнительные действия за игрока не нужно</t>
+  </si>
+  <si>
+    <t>Осирис, стоя на Сияющей Астральной Платформе, быстро активировал свой Хрономантический Переход, окружив себя мантией времени. В ультрабыстром перемещении он избежал ловушек, расставленных Теневым Хранителем, создавая вокруг себя иллюзию мельтешащих теней. Позиционируясь ловко вокруг врага, Осирис собрал звездную энергию в ладонях, приготавливаясь к магической атаке.
+Тем временем Теневой Хранитель, реагируя на неожиданный маневр Осириса, активировал свой Магический Щит, пытаясь устоять перед надвигающейся звездной энергией. Однако, не успев закончить защитное заклинание, он был вынужден отменить его, чтобы ответить на молниеносную атаку.
+Сияние звезд слилось с драконьей магией в руках Осириса, когда он выпустил мощный Звездный Резонанс. Вихрь световой энергии обрушился на Теневого Хранителя, пробиваясь сквозь его защиту. Оглушенный враг оказался в беззащитном положении, и блеск драконьего взгляда Осириса пронзил тьму, наполняя его новой уверенностью в борьбе против темных сил Эльдории.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вот текущая история боя, А вот фрагмент, на основании которого его нужно дополнить (верни только изменения в изначальной истории) (учти, что в PerformedActions нужно записывать только действия врагов, действия игрока записываются в PlayerActions):  </t>
+  </si>
+  <si>
+    <t>"PerformedActions": [
+    "Теневой Хранитель активирует свой Магический Щит, но отменяет его под давлением атаки Осириса",
+    "Осирис использует Звездный Резонанс против Теневого Хранителя"
+]
+"PlayerActions": [
+    "Осирис активирует Хрономантический Переход",
+    "Осирис готовит Звездный Резонанс"
+]
+"MainEvents": [
+    "Осирис готовится к Звездному Взрыву",
+    "Теневой Хранитель прерывает атаку магическим щитом",
+    "Хранитель вызывает тьму, окутывающую Осириса",
+    "Начало сражения с Теневым Хранителем",
+    "Осирис использует Хрономантический Переход, избегая ловушек",
+    "Теневой Хранитель отменяет Магический Щит под давлением атаки Осириса",
+    "Осирис готовит Звездный Резонанс",
+    "Осирис выпускает Звездный Резонанс, пробиваясь сквозь защиту Теневого Хранителя"
+]</t>
   </si>
 </sst>
 </file>
@@ -1594,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9746B0B3-BD14-45AF-A248-190EC1FFD653}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,9 +1723,10 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="4" max="7" width="30.7109375" customWidth="1"/>
     <col min="10" max="10" width="46.42578125" customWidth="1"/>
+    <col min="11" max="11" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1640,10 +1758,13 @@
         <v>33</v>
       </c>
       <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1662,11 +1783,11 @@
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1680,11 +1801,11 @@
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="405" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="405" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A29" si="0">A3+1</f>
         <v>3</v>
@@ -1704,11 +1825,11 @@
       <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1719,11 +1840,11 @@
       <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1740,11 +1861,11 @@
       <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1764,11 +1885,11 @@
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1785,11 +1906,11 @@
       <c r="I8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1809,11 +1930,11 @@
       <c r="I9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1836,11 +1957,11 @@
       <c r="J10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1877,11 +1998,11 @@
       <c r="J11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1913,11 +2034,11 @@
       <c r="J12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1940,11 +2061,11 @@
       <c r="J13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1967,11 +2088,11 @@
       <c r="J14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2004,11 +2125,11 @@
       <c r="J15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2031,11 +2152,11 @@
       <c r="J16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2071,7 +2192,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2102,7 +2223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2136,7 +2257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2167,7 +2288,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2202,56 +2323,176 @@
       <c r="J21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f>F22</f>
+        <v>Когда Осирис обратился к Мудрецам Звезд за знаниями о древних тайнах в Астральных Просторах, внезапно воздух наполнился таинственной аурой, а вокруг начал формироваться вихрь световой энергии. Мудрецы Звезд, стоявшие вокруг него, подняли руки в знак благословения, и звезды на их одеждах засветились ярче.
+Один из Мудрецов Звезд произнес: "Осирис, великий Звездный маг, ты достиг высших сфер знаний, но судьба Эльдории на волоске. Темные силы уже сгущаются вокруг нас, и лишь твоя магия может предотвратить их темное пробуждение."
+В этот момент Мудрецы Звезд подняли свои посохи вверх, создавая защитный барьер вокруг Осириса. Вихрь световой энергии, который он вызвал, стал контролируемым и начал вращаться вокруг него, словно звездные орбиты, создавая защитный щит.
+"Осирис, тебе предстоит пройти через испытания Звездного Резонанса, чтобы раскрыть истинный потенциал своей магии и спасти Эльдорию от тьмы. С этого момента ты несешь бремя не только своей судьбы, но и судьбы всего мира," объявил старший из Мудрецов Звезд.
+Игроку предстояло взять в руки свой Звездный посох, облачиться в Драконью чешую и взглянуть на светящийся вихрь световой энергии. Следы Звезд на его драконьей чешуе мерцали, свидетельствуя о его соединении с звездной энергией. Теперь, с магией и знаниями, полученными от Мудрецов Звезд, Осирис был готов к финальной битве, которая должна была решить судьбу Эльдории.</v>
+      </c>
+      <c r="D25" t="str">
+        <f>F24</f>
+        <v>{
+  "PossibleActions": [
+    "Применить Звездный Резонанс для создания магического барьера, защищающего от магических атак Теневого Хранителя.",
+    "Использовать Цветущее Прозрение, чтобы обнаружить уязвимости в магическом облике Теневого Хранителя и атаковать его слабые места.",
+    "Активировать Хрономантический Переход для быстрого перемещения вокруг Теневого Хранителя и избежания его ловушек, затем совершить магическую атаку."
+  ]
+}</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2267,7 +2508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286B1339-2F31-4E8C-B0A6-A8A3299A8401}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>